<commit_message>
Added Builder design pattern
</commit_message>
<xml_diff>
--- a/ClassDiagrams.xlsx
+++ b/ClassDiagrams.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7560" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleFactory" sheetId="2" r:id="rId1"/>
     <sheet name="FactoryMethod" sheetId="1" r:id="rId2"/>
     <sheet name="AbstractFactory" sheetId="3" r:id="rId3"/>
+    <sheet name="Builder" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>CLASS STRUCTURE</t>
   </si>
@@ -121,6 +122,57 @@
   </si>
   <si>
     <t>IronDoorFactory</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>pepperoni</t>
+  </si>
+  <si>
+    <t>lettuce</t>
+  </si>
+  <si>
+    <t>tomato</t>
+  </si>
+  <si>
+    <t>BurgerBuilder</t>
+  </si>
+  <si>
+    <t>add_pepperoni()</t>
+  </si>
+  <si>
+    <t>add_cheese()</t>
+  </si>
+  <si>
+    <t>add_lettuce()</t>
+  </si>
+  <si>
+    <t>add_tomato()</t>
+  </si>
+  <si>
+    <t>build_burger()</t>
+  </si>
+  <si>
+    <t>turns pepperoni flag to true</t>
+  </si>
+  <si>
+    <t>turns cheese flag to true</t>
+  </si>
+  <si>
+    <t>turns lettuce flasg to true</t>
+  </si>
+  <si>
+    <t>turns tomato flag to true</t>
+  </si>
+  <si>
+    <t>creates the burger class with the parameters supplied</t>
   </si>
 </sst>
 </file>
@@ -212,10 +264,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,22 +576,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="3" spans="1:14">
       <c r="C3" s="1" t="s">
@@ -629,16 +681,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="3" t="s">
@@ -717,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -732,20 +784,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="1" t="s">
@@ -775,7 +827,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -831,4 +883,128 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="E9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="E10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="E12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="E13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>